<commit_message>
Changed the way .xlsx is parsed
</commit_message>
<xml_diff>
--- a/Приложение 1. Список пассажиров (загрузите, демо).xlsx
+++ b/Приложение 1. Список пассажиров (загрузите, демо).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -124,7 +124,8 @@
     <t xml:space="preserve">Фитнес Клуб</t>
   </si>
   <si>
-    <t xml:space="preserve">2-я Инфекционная</t>
+    <t xml:space="preserve">Городская клиническая больница 1
+</t>
   </si>
   <si>
     <t xml:space="preserve">Фомичёв Нисон Проклович</t>
@@ -215,6 +216,10 @@
   </si>
   <si>
     <t xml:space="preserve">ИП “Сергеева Г.Л”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Городская клиническая больница 3
+</t>
   </si>
 </sst>
 </file>
@@ -336,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,6 +380,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -460,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -581,7 +590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
@@ -627,7 +636,7 @@
       <c r="O3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -819,7 +828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
@@ -865,8 +874,8 @@
       <c r="O8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="9" t="s">
-        <v>33</v>
+      <c r="P8" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>